<commit_message>
Update database and org feature 201712240341
</commit_message>
<xml_diff>
--- a/Docs/dictionarydata20171223.xlsx
+++ b/Docs/dictionarydata20171223.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="113">
   <si>
     <t>account</t>
   </si>
@@ -457,12 +457,28 @@
   <si>
     <t>studentmajor</t>
   </si>
+  <si>
+    <r>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Primary)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +526,45 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -531,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -580,11 +635,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -610,15 +676,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -642,13 +734,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>197</xdr:row>
+      <xdr:row>202</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>197</xdr:row>
+      <xdr:row>202</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1000,15 +1092,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955B5703-1EA2-4D8B-AF8E-DC97663BB94E}">
-  <dimension ref="A1:I198"/>
+  <dimension ref="A1:I203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1186,16 +1278,16 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -1210,13 +1302,13 @@
       <c r="H14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="6" t="s">
         <v>35</v>
       </c>
@@ -1229,7 +1321,7 @@
       <c r="H15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2119,7 +2211,7 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>24</v>
       </c>
@@ -2156,7 +2248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>31</v>
       </c>
@@ -2186,7 +2278,7 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>73</v>
       </c>
@@ -2194,7 +2286,7 @@
     <row r="90" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>1</v>
       </c>
@@ -2265,7 +2357,7 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>24</v>
       </c>
@@ -2303,16 +2395,16 @@
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="9" t="s">
+      <c r="A99" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D99" s="9" t="s">
+      <c r="D99" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E99" s="6" t="s">
@@ -2327,13 +2419,13 @@
       <c r="H99" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I99" s="9"/>
+      <c r="I99" s="10"/>
     </row>
     <row r="100" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="10"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
       <c r="E100" s="6" t="s">
         <v>54</v>
       </c>
@@ -2346,12 +2438,12 @@
       <c r="H100" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I100" s="10"/>
+      <c r="I100" s="11"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>76</v>
       </c>
@@ -2359,7 +2451,7 @@
     <row r="103" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2539,7 @@
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>24</v>
       </c>
@@ -2485,16 +2577,16 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B113" s="9" t="s">
+      <c r="B113" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D113" s="9" t="s">
+      <c r="D113" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E113" s="6" t="s">
@@ -2509,13 +2601,13 @@
       <c r="H113" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I113" s="9"/>
+      <c r="I113" s="10"/>
     </row>
     <row r="114" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
       <c r="E114" s="6" t="s">
         <v>79</v>
       </c>
@@ -2528,7 +2620,7 @@
       <c r="H114" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I114" s="10"/>
+      <c r="I114" s="11"/>
     </row>
     <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
@@ -2560,652 +2652,652 @@
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="117" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
+    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D119" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E119" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F119" s="3" t="s">
+      <c r="F119" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G119" s="3" t="s">
+      <c r="G119" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B120" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" s="16"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
+    </row>
+    <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" s="16">
+        <v>0</v>
+      </c>
+      <c r="E121" s="18"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+    </row>
+    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B122" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C122" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" s="16"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+    </row>
+    <row r="123" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B123" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" s="16"/>
+      <c r="E123" s="18"/>
+      <c r="F123" s="18"/>
+      <c r="G123" s="18"/>
+    </row>
+    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A125" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G127" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H127" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I127" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B128" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D128" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="F128" s="20">
+        <v>8</v>
+      </c>
+      <c r="G128" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H128" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I128" s="21"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="13"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+      <c r="G129" s="12"/>
+      <c r="H129" s="12"/>
+    </row>
+    <row r="130" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="4"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+    </row>
+    <row r="134" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+    </row>
+    <row r="135" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="4"/>
+      <c r="E135" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F140" s="6">
+        <v>0</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F141" s="6">
+        <v>0</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H141" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C120" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D120" s="4"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
-    </row>
-    <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D121" s="4">
-        <v>0</v>
-      </c>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
-    </row>
-    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B122" s="5" t="s">
+      <c r="C146" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+    </row>
+    <row r="147" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+    </row>
+    <row r="148" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D148" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+    </row>
+    <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" s="4">
+        <v>1</v>
+      </c>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A151" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C154" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D154" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F154" s="6">
+        <v>10</v>
+      </c>
+      <c r="G154" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H154" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I154" s="10"/>
+    </row>
+    <row r="155" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="11"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F155" s="6">
+        <v>10</v>
+      </c>
+      <c r="G155" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H155" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I155" s="11"/>
+    </row>
+    <row r="156" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F156" s="6">
+        <v>10</v>
+      </c>
+      <c r="G156" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H156" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I156" s="6"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D161" s="4"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+    </row>
+    <row r="162" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B162" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C122" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D122" s="4"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
-    </row>
-    <row r="123" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D123" s="4"/>
-      <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="6"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D128" s="4"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="6"/>
-    </row>
-    <row r="129" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D129" s="4"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
-    </row>
-    <row r="130" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D130" s="4"/>
-      <c r="E130" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C135" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D135" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E135" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F135" s="6">
-        <v>0</v>
-      </c>
-      <c r="G135" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H135" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I135" s="6"/>
-    </row>
-    <row r="136" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D136" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F136" s="6">
-        <v>0</v>
-      </c>
-      <c r="G136" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H136" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I136" s="6"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G140" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D141" s="4"/>
-      <c r="E141" s="6"/>
-      <c r="F141" s="6"/>
-      <c r="G141" s="6"/>
-    </row>
-    <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D142" s="4"/>
-      <c r="E142" s="6"/>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6"/>
-    </row>
-    <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B143" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D143" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="G143" s="6"/>
-    </row>
-    <row r="144" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D144" s="4">
-        <v>1</v>
-      </c>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F148" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G148" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H148" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E149" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F149" s="6">
-        <v>10</v>
-      </c>
-      <c r="G149" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H149" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I149" s="9"/>
-    </row>
-    <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="10"/>
-      <c r="B150" s="10"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F150" s="6">
-        <v>10</v>
-      </c>
-      <c r="G150" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H150" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I150" s="10"/>
-    </row>
-    <row r="151" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D151" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E151" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F151" s="6">
-        <v>10</v>
-      </c>
-      <c r="G151" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H151" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I151" s="6"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D156" s="4"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
-      <c r="G156" s="6"/>
-    </row>
-    <row r="157" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B157" s="5" t="s">
+      <c r="C162" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D162" s="4"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+    </row>
+    <row r="163" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D163" s="4"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+    </row>
+    <row r="164" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B164" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C157" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D157" s="4"/>
-      <c r="E157" s="6"/>
-      <c r="F157" s="6"/>
-      <c r="G157" s="6"/>
-    </row>
-    <row r="158" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D158" s="4"/>
-      <c r="E158" s="6"/>
-      <c r="F158" s="6"/>
-      <c r="G158" s="6"/>
-    </row>
-    <row r="159" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D159" s="4"/>
-      <c r="E159" s="6"/>
-      <c r="F159" s="6"/>
-      <c r="G159" s="6"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F163" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H163" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I163" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B164" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="C164" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D164" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E164" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F164" s="6">
-        <v>5</v>
-      </c>
-      <c r="G164" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H164" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I164" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="D164" s="4"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>97</v>
+    <row r="166" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3213,483 +3305,550 @@
     </row>
     <row r="168" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C168" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H168" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="I168" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D169" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F169" s="6">
+        <v>5</v>
+      </c>
+      <c r="G169" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H169" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D173" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E168" s="3" t="s">
+      <c r="E173" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F168" s="3" t="s">
+      <c r="F173" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G168" s="3" t="s">
+      <c r="G173" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="4" t="s">
+    <row r="174" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B174" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C169" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D169" s="4"/>
-      <c r="E169" s="6"/>
-      <c r="F169" s="6"/>
-      <c r="G169" s="6"/>
-    </row>
-    <row r="170" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="4" t="s">
+      <c r="C174" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D174" s="4"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+    </row>
+    <row r="175" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="B175" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C170" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D170" s="4"/>
-      <c r="E170" s="6"/>
-      <c r="F170" s="6"/>
-      <c r="G170" s="6"/>
-    </row>
-    <row r="171" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="4" t="s">
+      <c r="C175" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D175" s="4"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+    </row>
+    <row r="176" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B176" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C171" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D171" s="4"/>
-      <c r="E171" s="6"/>
-      <c r="F171" s="6"/>
-      <c r="G171" s="6"/>
-    </row>
-    <row r="172" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="4" t="s">
+      <c r="C176" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D176" s="4"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+    </row>
+    <row r="177" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B177" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C172" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D172" s="4"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
-      <c r="G172" s="6"/>
-    </row>
-    <row r="173" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="4" t="s">
+      <c r="C177" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D177" s="4"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+    </row>
+    <row r="178" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B178" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C173" s="6" t="s">
+      <c r="C178" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D173" s="7" t="s">
+      <c r="D178" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E173" s="6" t="s">
+      <c r="E178" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F173" s="6"/>
-      <c r="G173" s="6"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A175" s="8" t="s">
+      <c r="F178" s="6"/>
+      <c r="G178" s="6"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A180" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="3" t="s">
+    <row r="181" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B182" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C177" s="3" t="s">
+      <c r="C182" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D177" s="3" t="s">
+      <c r="D182" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E177" s="3" t="s">
+      <c r="E182" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F177" s="3" t="s">
+      <c r="F182" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G177" s="3" t="s">
+      <c r="G182" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H177" s="3" t="s">
+      <c r="H182" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I177" s="3" t="s">
+      <c r="I182" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="9" t="s">
+    <row r="183" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B178" s="9" t="s">
+      <c r="B183" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C178" s="9" t="s">
+      <c r="C183" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D178" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E178" s="6" t="s">
+      <c r="D183" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E183" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F178" s="6">
+      <c r="F183" s="6">
         <v>5</v>
       </c>
-      <c r="G178" s="6" t="s">
+      <c r="G183" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H178" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I178" s="9"/>
-    </row>
-    <row r="179" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="10"/>
-      <c r="B179" s="10"/>
-      <c r="C179" s="10"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="6" t="s">
+      <c r="H183" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I183" s="10"/>
+    </row>
+    <row r="184" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="11"/>
+      <c r="B184" s="11"/>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
+      <c r="E184" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F179" s="6">
+      <c r="F184" s="6">
         <v>5</v>
       </c>
-      <c r="G179" s="6" t="s">
+      <c r="G184" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H179" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I179" s="10"/>
-    </row>
-    <row r="180" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="6" t="s">
+      <c r="H184" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I184" s="11"/>
+    </row>
+    <row r="185" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B180" s="6" t="s">
+      <c r="B185" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C180" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D180" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E180" s="6" t="s">
+      <c r="C185" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E185" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F180" s="6">
+      <c r="F185" s="6">
         <v>5</v>
       </c>
-      <c r="G180" s="6" t="s">
+      <c r="G185" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H180" s="6" t="s">
+      <c r="H185" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I180" s="6"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="3" t="s">
+    <row r="188" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B184" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C184" s="3" t="s">
+      <c r="C189" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="D189" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E184" s="3" t="s">
+      <c r="E189" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F184" s="3" t="s">
+      <c r="F189" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G184" s="3" t="s">
+      <c r="G189" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="4" t="s">
+    <row r="190" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B185" s="5" t="s">
+      <c r="B190" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C185" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D185" s="4"/>
-      <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
-      <c r="G185" s="6"/>
-    </row>
-    <row r="186" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="4" t="s">
+      <c r="C190" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D190" s="4"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6"/>
+    </row>
+    <row r="191" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="B191" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C186" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D186" s="4"/>
-      <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
-      <c r="G186" s="6"/>
-    </row>
-    <row r="187" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="4" t="s">
+      <c r="C191" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D191" s="4"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="6"/>
+    </row>
+    <row r="192" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B187" s="5" t="s">
+      <c r="B192" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C187" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D187" s="4"/>
-      <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
-      <c r="G187" s="6"/>
-    </row>
-    <row r="188" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="4" t="s">
+      <c r="C192" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D192" s="4"/>
+      <c r="E192" s="6"/>
+      <c r="F192" s="6"/>
+      <c r="G192" s="6"/>
+    </row>
+    <row r="193" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B188" s="5" t="s">
+      <c r="B193" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C188" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D188" s="4"/>
-      <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
-      <c r="G188" s="6"/>
-    </row>
-    <row r="189" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="4" t="s">
+      <c r="C193" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D193" s="4"/>
+      <c r="E193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="6"/>
+    </row>
+    <row r="194" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="B194" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C189" s="6" t="s">
+      <c r="C194" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D189" s="7" t="s">
+      <c r="D194" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E189" s="6" t="s">
+      <c r="E194" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F189" s="6"/>
-      <c r="G189" s="6"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A191" s="8" t="s">
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A196" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="3" t="s">
+    <row r="197" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B198" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C193" s="3" t="s">
+      <c r="C198" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D193" s="3" t="s">
+      <c r="D198" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E193" s="3" t="s">
+      <c r="E198" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F198" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G193" s="3" t="s">
+      <c r="G198" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H193" s="3" t="s">
+      <c r="H198" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I193" s="3" t="s">
+      <c r="I198" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="9" t="s">
+    <row r="199" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B194" s="9" t="s">
+      <c r="B199" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C194" s="9" t="s">
+      <c r="C199" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D194" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E194" s="6" t="s">
+      <c r="D199" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E199" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F194" s="6">
+      <c r="F199" s="6">
         <v>5</v>
       </c>
-      <c r="G194" s="6" t="s">
+      <c r="G199" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H194" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I194" s="9"/>
-    </row>
-    <row r="195" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="10"/>
-      <c r="B195" s="10"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="10"/>
-      <c r="E195" s="6" t="s">
+      <c r="H199" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I199" s="10"/>
+    </row>
+    <row r="200" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="11"/>
+      <c r="B200" s="11"/>
+      <c r="C200" s="11"/>
+      <c r="D200" s="11"/>
+      <c r="E200" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F195" s="6">
+      <c r="F200" s="6">
         <v>5</v>
       </c>
-      <c r="G195" s="6" t="s">
+      <c r="G200" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H195" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I195" s="10"/>
-    </row>
-    <row r="196" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="6" t="s">
+      <c r="H200" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I200" s="11"/>
+    </row>
+    <row r="201" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B196" s="6" t="s">
+      <c r="B201" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C196" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D196" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E196" s="6" t="s">
+      <c r="C201" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E201" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F196" s="6">
+      <c r="F201" s="6">
         <v>5</v>
       </c>
-      <c r="G196" s="6" t="s">
+      <c r="G201" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H196" s="6" t="s">
+      <c r="H201" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I196" s="6"/>
-    </row>
-    <row r="197" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="11"/>
-    </row>
-    <row r="198" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="11"/>
+      <c r="I201" s="6"/>
+    </row>
+    <row r="202" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A202" s="9"/>
+    </row>
+    <row r="203" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A203" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="B178:B179"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="D178:D179"/>
-    <mergeCell ref="I178:I179"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="D194:D195"/>
-    <mergeCell ref="I194:I195"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="I99:I100"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="I154:I155"/>
     <mergeCell ref="A113:A114"/>
     <mergeCell ref="B113:B114"/>
     <mergeCell ref="C113:C114"/>
     <mergeCell ref="D113:D114"/>
     <mergeCell ref="I113:I114"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="I99:I100"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="B199:B200"/>
+    <mergeCell ref="C199:C200"/>
+    <mergeCell ref="D199:D200"/>
+    <mergeCell ref="I199:I200"/>
+    <mergeCell ref="A183:A184"/>
+    <mergeCell ref="B183:B184"/>
+    <mergeCell ref="C183:C184"/>
+    <mergeCell ref="D183:D184"/>
+    <mergeCell ref="I183:I184"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>